<commit_message>
corrected reserve economic and cycle sensitivity to apply to full reserve amounts
</commit_message>
<xml_diff>
--- a/Driver_Based_Model.xlsx
+++ b/Driver_Based_Model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\james\IFOA_WG_Capital_Models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chata\Desktop\3.6.2025\IFOA_WG_Capital_Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB67D866-41B9-46D8-87E1-7764139B20F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC10266-7E4D-438A-988D-B7730BE77B30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" firstSheet="7" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Underwriting" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -353,7 +353,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -372,6 +372,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -420,11 +427,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -436,10 +445,15 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma 2" xfId="3" xr:uid="{E3117B45-9F2F-4187-B39D-0515C465CACE}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -900,8 +914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -942,25 +956,25 @@
         <v>7</v>
       </c>
       <c r="B2" s="4">
-        <v>1887000000</v>
-      </c>
-      <c r="C2">
+        <v>2000000000</v>
+      </c>
+      <c r="C2" s="9">
         <v>10</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="9">
         <v>0.4</v>
       </c>
-      <c r="E2">
-        <v>21434272.127814323</v>
-      </c>
-      <c r="F2">
-        <v>6176213.1203094749</v>
-      </c>
-      <c r="G2">
-        <v>2.1665774084699665</v>
-      </c>
-      <c r="H2">
-        <v>387246722.29302722</v>
+      <c r="E2" s="9">
+        <v>2143427.213</v>
+      </c>
+      <c r="F2" s="9">
+        <v>6176213.1200000001</v>
+      </c>
+      <c r="G2" s="9">
+        <v>2.1665774080000002</v>
+      </c>
+      <c r="H2" s="9">
+        <v>38724672.229999997</v>
       </c>
       <c r="J2" s="6"/>
     </row>
@@ -969,25 +983,25 @@
         <v>8</v>
       </c>
       <c r="B3" s="4">
-        <v>3050000000</v>
-      </c>
-      <c r="C3">
+        <v>1000000000</v>
+      </c>
+      <c r="C3" s="9">
         <v>10</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="9">
         <v>0.4</v>
       </c>
-      <c r="E3">
-        <v>12123239.056982597</v>
-      </c>
-      <c r="F3">
-        <v>47594601.571695596</v>
-      </c>
-      <c r="G3">
-        <v>6.9249013413173603</v>
-      </c>
-      <c r="H3">
-        <v>163179220.0779942</v>
+      <c r="E3" s="9">
+        <v>12123239.060000001</v>
+      </c>
+      <c r="F3" s="9">
+        <v>47594601.57</v>
+      </c>
+      <c r="G3" s="9">
+        <v>6.924901341</v>
+      </c>
+      <c r="H3" s="9">
+        <v>16317922.01</v>
       </c>
       <c r="J3" s="6"/>
     </row>
@@ -996,25 +1010,25 @@
         <v>9</v>
       </c>
       <c r="B4" s="4">
-        <v>1887000000</v>
-      </c>
-      <c r="C4">
+        <v>1000000000</v>
+      </c>
+      <c r="C4" s="9">
         <v>10</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="9">
         <v>0.4</v>
       </c>
-      <c r="E4">
-        <v>10012524.013125015</v>
-      </c>
-      <c r="F4">
-        <v>39212459.978124946</v>
-      </c>
-      <c r="G4">
-        <v>6.9243640207395618</v>
-      </c>
-      <c r="H4">
-        <v>111057130.6888963</v>
+      <c r="E4" s="9">
+        <v>10012524.01</v>
+      </c>
+      <c r="F4" s="9">
+        <v>39212459.979999997</v>
+      </c>
+      <c r="G4" s="9">
+        <v>6.9243640209999997</v>
+      </c>
+      <c r="H4" s="9">
+        <v>11105713.07</v>
       </c>
       <c r="J4" s="6"/>
     </row>
@@ -1057,7 +1071,7 @@
         <v>30</v>
       </c>
       <c r="B3">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
     </row>
   </sheetData>
@@ -1070,7 +1084,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1091,7 +1105,7 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1099,7 +1113,7 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>0.7</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1120,7 +1134,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1152,10 +1166,10 @@
         <v>0.02</v>
       </c>
       <c r="C2">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="D2">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1166,10 +1180,10 @@
         <v>0.02</v>
       </c>
       <c r="C3">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="D3">
-        <v>1.5</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1182,7 +1196,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M37" sqref="M37"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1199,24 +1213,24 @@
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2">
-        <v>1.5</v>
+      <c r="B2" s="9">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3">
-        <v>1</v>
+      <c r="B3" s="9">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4">
-        <v>2</v>
+      <c r="B4" s="9">
+        <v>2.5</v>
       </c>
     </row>
   </sheetData>
@@ -1229,7 +1243,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1260,10 +1274,10 @@
         <v>0.25</v>
       </c>
       <c r="C2" s="4">
-        <v>10000000</v>
+        <v>5000000</v>
       </c>
       <c r="D2" s="4">
-        <v>100000000</v>
+        <v>200000000</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1274,10 +1288,10 @@
         <v>0.25</v>
       </c>
       <c r="C3" s="4">
-        <v>10000000</v>
+        <v>5000000</v>
       </c>
       <c r="D3" s="4">
-        <v>100000000</v>
+        <v>200000000</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1288,10 +1302,10 @@
         <v>0.3</v>
       </c>
       <c r="C4" s="4">
-        <v>10000000</v>
+        <v>5000000</v>
       </c>
       <c r="D4" s="4">
-        <v>100000000</v>
+        <v>200000000</v>
       </c>
     </row>
   </sheetData>
@@ -1303,9 +1317,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40B7C559-26D8-4DC7-B282-BB012F5AB4AC}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1334,7 +1346,7 @@
         <v>100000000</v>
       </c>
       <c r="C2" s="4">
-        <v>100000000</v>
+        <v>50000000</v>
       </c>
       <c r="E2" s="1"/>
     </row>
@@ -1346,7 +1358,7 @@
         <v>500000000</v>
       </c>
       <c r="C3" s="4">
-        <v>200000000</v>
+        <v>100000000</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1357,7 +1369,7 @@
         <v>300000000</v>
       </c>
       <c r="C4" s="4">
-        <v>700000000</v>
+        <v>350000000</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1368,7 +1380,7 @@
         <v>1000000000</v>
       </c>
       <c r="C5" s="4">
-        <v>1000000000</v>
+        <v>500000000</v>
       </c>
     </row>
   </sheetData>
@@ -1380,9 +1392,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E43E834F-4823-49A8-91C2-CFB2B90CFB76}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1690,8 +1700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0011351-CB19-4B85-A86D-FE846EF8FA28}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M46" sqref="M46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2107,7 +2117,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2133,10 +2143,10 @@
         <v>7</v>
       </c>
       <c r="B2" s="4">
-        <v>5000000000</v>
-      </c>
-      <c r="C2">
-        <v>0.2</v>
+        <v>2000000000</v>
+      </c>
+      <c r="C2" s="9">
+        <v>0.1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2146,8 +2156,8 @@
       <c r="B3" s="4">
         <v>1000000000</v>
       </c>
-      <c r="C3">
-        <v>0.2</v>
+      <c r="C3" s="9">
+        <v>0.1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2155,10 +2165,10 @@
         <v>9</v>
       </c>
       <c r="B4" s="4">
-        <v>8000000000</v>
-      </c>
-      <c r="C4">
-        <v>0.5</v>
+        <v>1000000000</v>
+      </c>
+      <c r="C4" s="9">
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>
@@ -2171,11 +2181,12 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="33.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.42578125" bestFit="1" customWidth="1"/>
@@ -2233,8 +2244,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2273,7 +2284,7 @@
         <v>16</v>
       </c>
       <c r="C3">
-        <v>0.02</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2339,7 +2350,7 @@
         <v>57</v>
       </c>
       <c r="C9">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2349,8 +2360,8 @@
       <c r="B10" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="4">
-        <v>14000000000</v>
+      <c r="C10" s="7">
+        <v>4000000000</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2383,7 +2394,7 @@
         <v>56</v>
       </c>
       <c r="C13">
-        <v>-2</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -2394,7 +2405,7 @@
         <v>58</v>
       </c>
       <c r="C14">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2405,7 +2416,7 @@
         <v>14</v>
       </c>
       <c r="C15">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -2416,7 +2427,7 @@
         <v>62</v>
       </c>
       <c r="C16">
-        <v>-1</v>
+        <v>-0.3</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2451,7 +2462,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2527,7 +2538,7 @@
         <v>-0.3</v>
       </c>
       <c r="C5">
-        <v>-0.75</v>
+        <v>0.5</v>
       </c>
       <c r="D5">
         <v>0.1</v>
@@ -2541,16 +2552,16 @@
         <v>86</v>
       </c>
       <c r="B6">
-        <v>0.2</v>
+        <v>-0.3</v>
       </c>
       <c r="C6">
         <v>0.5</v>
       </c>
       <c r="D6">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E6">
-        <v>-0.5</v>
+        <v>0.9</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -2561,7 +2572,7 @@
         <v>87</v>
       </c>
       <c r="B7">
-        <v>0.5</v>
+        <v>-0.1</v>
       </c>
       <c r="C7">
         <v>-0.1</v>
@@ -2614,7 +2625,7 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -2625,7 +2636,7 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>-0.1</v>
+        <v>-0.5</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -2636,7 +2647,7 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>-1.5</v>
+        <v>-2.5</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -2652,7 +2663,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2687,13 +2698,13 @@
         <v>-0.02</v>
       </c>
       <c r="C2">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="D2">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="E2">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2704,13 +2715,13 @@
         <v>-0.02</v>
       </c>
       <c r="C3">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="D3">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="E3">
-        <v>1.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2729,15 +2740,20 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -2748,40 +2764,40 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
       <c r="B2" t="s">
         <v>23</v>
       </c>
-      <c r="C2">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C2" s="8">
+        <v>2.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
       <c r="B3" t="s">
         <v>24</v>
       </c>
-      <c r="C3">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C3" s="8">
+        <v>5.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
       <c r="B4" t="s">
         <v>25</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="8">
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -2789,10 +2805,10 @@
         <v>17</v>
       </c>
       <c r="C5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -2800,10 +2816,10 @@
         <v>18</v>
       </c>
       <c r="C6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>66</v>
       </c>
@@ -2814,7 +2830,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>66</v>
       </c>
@@ -2825,7 +2841,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>66</v>
       </c>
@@ -2836,7 +2852,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>66</v>
       </c>
@@ -2847,7 +2863,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>66</v>
       </c>
@@ -2858,7 +2874,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>66</v>
       </c>
@@ -2869,7 +2885,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>66</v>
       </c>
@@ -2880,7 +2896,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>66</v>
       </c>
@@ -2891,7 +2907,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>66</v>
       </c>
@@ -2902,7 +2918,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>66</v>
       </c>
@@ -2912,8 +2928,9 @@
       <c r="C16" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -2924,7 +2941,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>77</v>
       </c>
@@ -2935,7 +2952,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>77</v>
       </c>
@@ -2945,8 +2962,9 @@
       <c r="C19">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I19" s="2"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>77</v>
       </c>
@@ -2957,7 +2975,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>77</v>
       </c>
@@ -2968,7 +2986,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>77</v>
       </c>
@@ -2979,7 +2997,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>77</v>
       </c>
@@ -2990,7 +3008,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>77</v>
       </c>
@@ -3001,7 +3019,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>77</v>
       </c>
@@ -3011,8 +3029,11 @@
       <c r="C25">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>77</v>
       </c>
@@ -3022,6 +3043,9 @@
       <c r="C26">
         <v>0.1</v>
       </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G28" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3033,7 +3057,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3067,7 +3091,7 @@
         <v>28</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>